<commit_message>
Complete second log entry for 03/16/2020 @ 19:30
</commit_message>
<xml_diff>
--- a/PWM_CALCULATOR.xlsx
+++ b/PWM_CALCULATOR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\CapstoneLogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CapstoneLogs\CapstoneLogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E8BAC4-591D-4301-9613-9E6EBB0EA51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6146DE3-9341-4527-A7EF-2E496853A2B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40950" yWindow="45" windowWidth="28800" windowHeight="15555" xr2:uid="{4CEE8F0A-EC37-4B1C-ADC9-6A9AD9C93362}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25545" windowHeight="15750" xr2:uid="{4CEE8F0A-EC37-4B1C-ADC9-6A9AD9C93362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Input Frequency</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>CCR2</t>
+  </si>
+  <si>
+    <t>Desired Frequency (Hz)</t>
+  </si>
+  <si>
+    <t>ARR</t>
   </si>
 </sst>
 </file>
@@ -170,13 +176,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -494,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9C6E62-45C1-4646-9B8C-AB67EEE40201}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,7 +539,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>840</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -540,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
@@ -555,9 +563,6 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -577,9 +582,317 @@
       </c>
       <c r="B7" s="3">
         <f>B4*B5</f>
+        <v>500</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>20</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>40</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>50</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>60</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>70</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>80</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>90</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>100</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>200</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>300</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>400</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>500</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>600</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>700</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>800</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>900</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>1100</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>1200</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>1300</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>1400</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>1500</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>1600</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>1700</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>1800</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>1900</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>2000</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>2500</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>3000</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>3500</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>4000</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>4500</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>5000</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>6000</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>7000</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>8000</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>9000</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>